<commit_message>
fix Excel template in Swedish. Fixed export Excel file extension to .xlsx
</commit_message>
<xml_diff>
--- a/src/assets/hanterade_konton.xlsx
+++ b/src/assets/hanterade_konton.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Given name</t>
+    <t xml:space="preserve">Förnamn</t>
   </si>
   <si>
-    <t xml:space="preserve">Surname</t>
+    <t xml:space="preserve">Efternamn </t>
   </si>
 </sst>
 </file>
@@ -137,10 +137,10 @@
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.0078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>